<commit_message>
Add cosmetic changes to the P&G report
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1207D5A0-643B-484A-A22E-C6F12F5D0272}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="24030" yWindow="-9890" windowWidth="24310" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -43,12 +49,6 @@
     <t>8 or 9</t>
   </si>
   <si>
-    <t>Dec 1, 2021</t>
-  </si>
-  <si>
-    <t>Dec 1, 2022</t>
-  </si>
-  <si>
     <t>Dec 1, 2023</t>
   </si>
   <si>
@@ -75,12 +75,18 @@
   <si>
     <t>Jan 2020 - Dec 2024</t>
   </si>
+  <si>
+    <t>Dec 1, 2021*</t>
+  </si>
+  <si>
+    <t>Dec 1, 2022*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +235,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +287,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,14 +480,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,74 +508,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -527,8 +584,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8503a06cff0f795d8db980f97ccdc33c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="45aa48cc5486c3369db2010050ce8f74" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d081261b7e6525d637bb9041e4a092fe">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afb925730929aa803742fae0db08f187" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
     <xsd:import namespace="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
     <xsd:element name="properties">
@@ -552,6 +630,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:UpdatedtoZOHO" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -626,6 +705,14 @@
     <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UpdatedtoZOHO" ma:index="24" nillable="true" ma:displayName="Updated to ZOHO" ma:description="Buildings module updates with Utility Provider and who pays" ma:format="Dropdown" ma:internalName="UpdatedtoZOHO">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Yes"/>
+          <xsd:enumeration value="No"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -769,19 +856,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5613E08-899C-49CC-8E73-A0C115239918}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB2550F7-CDE4-4FFF-9344-9206B507C5C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edit EBEWE Dates file to account for new EBEWE exemption changes
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1207D5A0-643B-484A-A22E-C6F12F5D0272}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FF00CC5-E81F-4276-A303-F2322C9E1779}"/>
   <bookViews>
-    <workbookView xWindow="24030" yWindow="-9890" windowWidth="24310" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-12430" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,32 +61,32 @@
     <t>Every 5 years thereafter</t>
   </si>
   <si>
-    <t>Jan 2016 - Dec 2020</t>
-  </si>
-  <si>
-    <t>Jan 2017 - Dec 2021</t>
-  </si>
-  <si>
-    <t>Jan 2018 - Dec 2022</t>
-  </si>
-  <si>
-    <t>Jan 2019 - Dec 2023</t>
-  </si>
-  <si>
-    <t>Jan 2020 - Dec 2024</t>
-  </si>
-  <si>
-    <t>Dec 1, 2021*</t>
-  </si>
-  <si>
-    <t>Dec 1, 2022*</t>
+    <t>Dec 1, 2022</t>
+  </si>
+  <si>
+    <t>Dec 1, 2021</t>
+  </si>
+  <si>
+    <t>Data must not be older than 12/1/2016</t>
+  </si>
+  <si>
+    <t>Data must not be older than 12/1/2017</t>
+  </si>
+  <si>
+    <t>Data must not be older than 12/1/2018</t>
+  </si>
+  <si>
+    <t>Data must not be older than 12/1/2019</t>
+  </si>
+  <si>
+    <t>Data must not be older than 12/1/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +98,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,9 +167,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,9 +207,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,26 +242,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,26 +277,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -484,17 +456,17 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,35 +480,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -547,10 +519,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -561,10 +533,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -575,36 +547,17 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d081261b7e6525d637bb9041e4a092fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afb925730929aa803742fae0db08f187" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
@@ -856,26 +809,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
-    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB2550F7-CDE4-4FFF-9344-9206B507C5C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -892,4 +847,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove the comp period column
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FF00CC5-E81F-4276-A303-F2322C9E1779}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3612DD05-CB39-4A8E-AA63-20A17729E691}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-12430" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>LAST DIGIT OF LADBS BUILDING ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>SUBSEQUENT DUE DATE</t>
   </si>
   <si>
-    <t>ENERGY CONSUMPTION COMPARATIVE PERIOD</t>
-  </si>
-  <si>
     <t>0 or 1</t>
   </si>
   <si>
@@ -65,21 +62,6 @@
   </si>
   <si>
     <t>Dec 1, 2021</t>
-  </si>
-  <si>
-    <t>Data must not be older than 12/1/2016</t>
-  </si>
-  <si>
-    <t>Data must not be older than 12/1/2017</t>
-  </si>
-  <si>
-    <t>Data must not be older than 12/1/2018</t>
-  </si>
-  <si>
-    <t>Data must not be older than 12/1/2019</t>
-  </si>
-  <si>
-    <t>Data must not be older than 12/1/2020</t>
   </si>
 </sst>
 </file>
@@ -453,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,7 +448,7 @@
     <col min="4" max="4" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,78 +458,60 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -558,8 +522,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d081261b7e6525d637bb9041e4a092fe">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afb925730929aa803742fae0db08f187" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd03adb9b17da248d6b02fb7f1aae572">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d2462fb3760918c6429aa1eacc387c6" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
     <xsd:import namespace="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
     <xsd:element name="properties">
@@ -584,6 +569,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:UpdatedtoZOHO" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -666,6 +652,11 @@
           <xsd:enumeration value="Yes"/>
           <xsd:enumeration value="No"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -809,55 +800,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB2550F7-CDE4-4FFF-9344-9206B507C5C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
-    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -866,4 +809,16 @@
     <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171EB9C6-B3A9-41BE-A4B5-220CFF7634BC}"/>
 </file>
</xml_diff>

<commit_message>
Edit ebewe compliance table
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3612DD05-CB39-4A8E-AA63-20A17729E691}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32F504FF-ADDD-4DCA-81D6-9E495DBE220E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35950" yWindow="-10800" windowWidth="17260" windowHeight="9950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>LAST DIGIT OF LADBS BUILDING ID</t>
   </si>
   <si>
-    <t>COMPLIANCE DUE DATE</t>
-  </si>
-  <si>
-    <t>SUBSEQUENT DUE DATE</t>
-  </si>
-  <si>
     <t>0 or 1</t>
   </si>
   <si>
@@ -55,13 +49,49 @@
     <t>Dec 1, 2025</t>
   </si>
   <si>
-    <t>Every 5 years thereafter</t>
-  </si>
-  <si>
     <t>Dec 1, 2022</t>
   </si>
   <si>
     <t>Dec 1, 2021</t>
+  </si>
+  <si>
+    <t>INITIAL COMPLIANCE DUE DATE</t>
+  </si>
+  <si>
+    <t>INITIAL COMPARATIVE PERIOD</t>
+  </si>
+  <si>
+    <t>Dec 1, 2016 - Dec 1, 2021</t>
+  </si>
+  <si>
+    <t>Dec 1, 2017 - Dec 1, 2022</t>
+  </si>
+  <si>
+    <t>Dec 1, 2018 - Dec 1, 2023</t>
+  </si>
+  <si>
+    <t>Dec 1, 2019 - Dec 1, 2024</t>
+  </si>
+  <si>
+    <t>Dec 1, 2020 - Dec 1, 2025</t>
+  </si>
+  <si>
+    <t>NEXT COMPLIANCE DUE DATE</t>
+  </si>
+  <si>
+    <t>Dec 1, 2026</t>
+  </si>
+  <si>
+    <t>Dec 1, 2027</t>
+  </si>
+  <si>
+    <t>Dec 1, 2028</t>
+  </si>
+  <si>
+    <t>Dec 1, 2029</t>
+  </si>
+  <si>
+    <t>Dec 1, 2030</t>
   </si>
 </sst>
 </file>
@@ -126,11 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,83 +466,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -522,6 +573,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
@@ -531,15 +591,6 @@
     <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -801,6 +852,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -811,14 +870,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171EB9C6-B3A9-41BE-A4B5-220CFF7634BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171EB9C6-B3A9-41BE-A4B5-220CFF7634BC}"/>
 </file>
</xml_diff>

<commit_message>
Edit ebewe dates table to add reissued due dates
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyleg\Green EconoMe\Shared - Documents\Green Econome Business\Software\GitHub\Progress-And-Goals\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_A4CB59F278014094D88DBBD452BDF15BEED42390" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32F504FF-ADDD-4DCA-81D6-9E495DBE220E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35950" yWindow="-10800" windowWidth="17260" windowHeight="9950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,24 +49,12 @@
     <t>Dec 1, 2025</t>
   </si>
   <si>
-    <t>Dec 1, 2022</t>
-  </si>
-  <si>
-    <t>Dec 1, 2021</t>
-  </si>
-  <si>
     <t>INITIAL COMPLIANCE DUE DATE</t>
   </si>
   <si>
     <t>INITIAL COMPARATIVE PERIOD</t>
   </si>
   <si>
-    <t>Dec 1, 2016 - Dec 1, 2021</t>
-  </si>
-  <si>
-    <t>Dec 1, 2017 - Dec 1, 2022</t>
-  </si>
-  <si>
     <t>Dec 1, 2018 - Dec 1, 2023</t>
   </si>
   <si>
@@ -92,6 +80,74 @@
   </si>
   <si>
     <t>Dec 1, 2030</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dec 1, 2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sept 7, 2023*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dec 1, 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sept 7, 2023*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dec 1, 2016 - Dec 1, 2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sept 1, 2018 - Sept 1, 2023*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dec 1, 2017 - Dec 1, 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sept 1, 2018 - Sept 1, 2023*</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -156,12 +212,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +528,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,41 +545,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -531,10 +590,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -545,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -559,10 +618,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for new ebewe dates and compliance periods
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyleg\Green EconoMe\Shared - Documents\Green Econome Business\Software\GitHub\Progress-And-Goals\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB55030A-EC01-4AD6-913B-B949B63849C9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-11570" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,6 @@
     <t>8 or 9</t>
   </si>
   <si>
-    <t>Dec 1, 2023</t>
-  </si>
-  <si>
-    <t>Dec 1, 2024</t>
-  </si>
-  <si>
     <t>Dec 1, 2025</t>
   </si>
   <si>
@@ -55,12 +49,6 @@
     <t>INITIAL COMPARATIVE PERIOD</t>
   </si>
   <si>
-    <t>Dec 1, 2018 - Dec 1, 2023</t>
-  </si>
-  <si>
-    <t>Dec 1, 2019 - Dec 1, 2024</t>
-  </si>
-  <si>
     <t>Dec 1, 2020 - Dec 1, 2025</t>
   </si>
   <si>
@@ -82,72 +70,28 @@
     <t>Dec 1, 2030</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Dec 1, 2021
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sept 7, 2023*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dec 1, 2022
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sept 7, 2023*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dec 1, 2016 - Dec 1, 2021
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sept 1, 2018 - Sept 1, 2023*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dec 1, 2017 - Dec 1, 2022
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sept 1, 2018 - Sept 1, 2023*</t>
-    </r>
+    <t>Dec 1, 2031</t>
+  </si>
+  <si>
+    <t>Dec 1, 2032</t>
+  </si>
+  <si>
+    <t>Dec 1, 2033</t>
+  </si>
+  <si>
+    <t>Dec 1, 2034</t>
+  </si>
+  <si>
+    <t>Dec 1, 2011 - Dec 1, 2026</t>
+  </si>
+  <si>
+    <t>Dec 1, 2022 - Dec 1, 2027</t>
+  </si>
+  <si>
+    <t>Dec 1, 2023 - Dec 1, 2028</t>
+  </si>
+  <si>
+    <t>Dec 1, 2024 - Dec 1, 2029</t>
   </si>
 </sst>
 </file>
@@ -212,13 +156,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -528,7 +475,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,83 +492,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -632,15 +579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
@@ -650,6 +588,15 @@
     <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -911,20 +858,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
     <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Change column header for due date
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB55030A-EC01-4AD6-913B-B949B63849C9}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D82A185-E927-4E4C-A3FA-2696384906E0}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-11570" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Dec 1, 2025</t>
   </si>
   <si>
-    <t>INITIAL COMPLIANCE DUE DATE</t>
-  </si>
-  <si>
     <t>INITIAL COMPARATIVE PERIOD</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Dec 1, 2024 - Dec 1, 2029</t>
+  </si>
+  <si>
+    <t>CURRENT COMPLIANCE DUE DATE</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,13 +506,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,13 +520,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,13 +534,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,13 +548,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,10 +565,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -591,17 +591,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd03adb9b17da248d6b02fb7f1aae572">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d2462fb3760918c6429aa1eacc387c6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="454a1fd8f3b7097e5644e879d208548d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="204506395bebcb762eeb57b8b85e60f6" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
     <xsd:import namespace="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
     <xsd:element name="properties">
@@ -627,6 +618,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:UpdatedtoZOHO" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -714,6 +706,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="26" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -857,6 +854,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
   <ds:schemaRefs>
@@ -869,15 +875,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171EB9C6-B3A9-41BE-A4B5-220CFF7634BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39E22535-3E24-4183-B5E3-5D4A54A1E8DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -893,4 +891,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add comment about compliance cycles
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D82A185-E927-4E4C-A3FA-2696384906E0}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C294A321-769B-4A29-A069-143673383674}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-11570" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,15 +37,9 @@
     <t>6 or 7</t>
   </si>
   <si>
-    <t>8 or 9</t>
-  </si>
-  <si>
     <t>Dec 1, 2025</t>
   </si>
   <si>
-    <t>INITIAL COMPARATIVE PERIOD</t>
-  </si>
-  <si>
     <t>Dec 1, 2020 - Dec 1, 2025</t>
   </si>
   <si>
@@ -92,6 +86,12 @@
   </si>
   <si>
     <t>CURRENT COMPLIANCE DUE DATE</t>
+  </si>
+  <si>
+    <t>8 or 9*</t>
+  </si>
+  <si>
+    <t>5-YEAR COMPARATIVE PERIOD</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,13 +492,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,13 +506,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,13 +520,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,13 +534,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,27 +548,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -579,18 +579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="454a1fd8f3b7097e5644e879d208548d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="204506395bebcb762eeb57b8b85e60f6" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
@@ -854,6 +842,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -864,17 +864,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
-    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39E22535-3E24-4183-B5E3-5D4A54A1E8DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -893,6 +882,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix comparative period year
</commit_message>
<xml_diff>
--- a/Resources/EBEWE Dates.xlsx
+++ b/Resources/EBEWE Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greeneconome.sharepoint.com/sites/Shared13/Shared Documents/Green Econome Business/Software/GitHub/Progress-And-Goals/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C294A321-769B-4A29-A069-143673383674}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{A2F04A86-C4A8-43C9-A519-072D0541B5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A2EFB68-1960-495C-8C40-C9DAB834A7F4}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-11570" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25330" yWindow="-9860" windowWidth="24770" windowHeight="18990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Dec 1, 2034</t>
   </si>
   <si>
-    <t>Dec 1, 2011 - Dec 1, 2026</t>
-  </si>
-  <si>
     <t>Dec 1, 2022 - Dec 1, 2027</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>5-YEAR COMPARATIVE PERIOD</t>
+  </si>
+  <si>
+    <t>Dec 1, 2021 - Dec 1, 2026</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
@@ -523,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -537,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -551,7 +551,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -579,6 +579,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007272FE551E20B741B46584F6EC656D2C" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="454a1fd8f3b7097e5644e879d208548d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0654f59d-bfad-4581-b70e-efdb5ac9d032" xmlns:ns3="0ab20313-a906-44ea-b7dc-a2b5971d84e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="204506395bebcb762eeb57b8b85e60f6" ns2:_="" ns3:_="">
     <xsd:import namespace="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
@@ -842,18 +854,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0ab20313-a906-44ea-b7dc-a2b5971d84e9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UpdatedtoZOHO xmlns="0654f59d-bfad-4581-b70e-efdb5ac9d032" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -864,6 +864,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
+    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39E22535-3E24-4183-B5E3-5D4A54A1E8DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -882,17 +893,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D11DCA-5C72-484C-BE52-0FFBD0DA8CD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ab20313-a906-44ea-b7dc-a2b5971d84e9"/>
-    <ds:schemaRef ds:uri="0654f59d-bfad-4581-b70e-efdb5ac9d032"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AF59AAE-A5A2-4B3A-AAEB-22132EEF7693}">
   <ds:schemaRefs>

</xml_diff>